<commit_message>
A bit more stable
</commit_message>
<xml_diff>
--- a/src/assets/Casting Replies Log.xlsx
+++ b/src/assets/Casting Replies Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Opera Downloads\Casting Replies Webpage\casting-log\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70B4761-76B4-4E86-A165-282377579460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCE686-1C2A-4BEB-AA5C-AC8CFB056AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -125,9 +125,6 @@
     <t>abhaya_deshmukh</t>
   </si>
   <si>
-    <t>Sameer Virutkar</t>
-  </si>
-  <si>
     <t>+91 90216 91481</t>
   </si>
   <si>
@@ -263,7 +260,49 @@
     <t>Phone</t>
   </si>
   <si>
+    <t>WhatsApp Image 2025-04-15 at 10.55.24_4b93487f.jpg</t>
+  </si>
+  <si>
     <t>IMG-20250415-WA0004.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 10.36.18_8c39dc73.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 10.46.36_36c4cda7.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 10.31.22_12a5858c.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 10.40.30_86d67314.jpg</t>
+  </si>
+  <si>
+    <t>Screenshot 2025-04-16 162757.png</t>
+  </si>
+  <si>
+    <t>IMG-20250101-WA0010.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 12.13.34_2bc9c20c.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 12.17.45_f8d38ca8.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 12.25.57_e77b436a.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 19.22.07_d840a353.jpg</t>
+  </si>
+  <si>
+    <t>IMG-20250415-WA0046.jpg</t>
+  </si>
+  <si>
+    <t>WhatsApp Image 2025-04-15 at 19.47.13_51ddcab9.jpg</t>
+  </si>
+  <si>
+    <t>IMG-20250416-WA0005.jpg</t>
   </si>
 </sst>
 </file>
@@ -738,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -770,7 +809,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -791,7 +830,7 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -857,6 +896,9 @@
       <c r="J3" t="s">
         <v>20</v>
       </c>
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -882,6 +924,9 @@
       <c r="J4" t="s">
         <v>23</v>
       </c>
+      <c r="L4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -912,6 +957,9 @@
       <c r="K5" t="s">
         <v>28</v>
       </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -919,7 +967,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>17</v>
@@ -928,19 +976,22 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="J6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>33</v>
       </c>
-      <c r="K6" t="s">
-        <v>34</v>
+      <c r="L6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -949,18 +1000,21 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="7"/>
+      <c r="L7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -968,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>17</v>
@@ -977,15 +1031,18 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" s="7"/>
       <c r="J8" t="s">
         <v>27</v>
       </c>
+      <c r="L8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -993,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>10</v>
@@ -1002,17 +1059,20 @@
         <v>22</v>
       </c>
       <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>40</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
       </c>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1020,7 +1080,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>17</v>
@@ -1029,22 +1089,22 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>45</v>
       </c>
       <c r="J10" t="s">
         <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1053,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>17</v>
@@ -1062,22 +1122,25 @@
         <v>24</v>
       </c>
       <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="I11">
         <v>66</v>
       </c>
       <c r="J11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" t="s">
         <v>50</v>
       </c>
-      <c r="K11" t="s">
-        <v>51</v>
+      <c r="L11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1086,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>10</v>
@@ -1095,17 +1158,20 @@
         <v>47</v>
       </c>
       <c r="E12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="J12" t="s">
         <v>27</v>
       </c>
+      <c r="L12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1113,18 +1179,21 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H13" s="7"/>
+      <c r="L13" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1132,7 +1201,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>10</v>
@@ -1141,19 +1210,22 @@
         <v>12</v>
       </c>
       <c r="E14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="J14" t="s">
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="L14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1162,18 +1234,21 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H15" s="7"/>
+      <c r="L15" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1181,29 +1256,32 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H16" s="7"/>
       <c r="J16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>ROW() - ROW(Table1[[#Headers],[No]])</f>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f>ROW() - ROW(Table1[[#Headers],[No]])</f>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>66</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>10</v>
@@ -1212,20 +1290,20 @@
         <v>30</v>
       </c>
       <c r="E17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>ROW() - ROW(Table1[[#Headers],[No]])</f>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f>ROW() - ROW(Table1[[#Headers],[No]])</f>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>68</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>17</v>
@@ -1234,16 +1312,19 @@
         <v>22</v>
       </c>
       <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="7" t="s">
+      <c r="J18" t="s">
         <v>70</v>
       </c>
-      <c r="J18" t="s">
-        <v>71</v>
+      <c r="L18" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>